<commit_message>
v3.0 update FCI 27/1/2023
</commit_message>
<xml_diff>
--- a/backend/src/excel_handler/files/AGRO.xlsx
+++ b/backend/src/excel_handler/files/AGRO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,115 +439,153 @@
           <t>06-01-2023</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>13-01-2023</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>total</t>
+          <t>1822 Raices Valores Negociables</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2034666.84</v>
+        <v>27202.22</v>
+      </c>
+      <c r="C2" t="n">
+        <v>26329.59</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>avg</t>
+          <t>Alpha Acciones</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>226074.09</v>
+        <v>370309.86</v>
+      </c>
+      <c r="C3" t="n">
+        <v>368466.44</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>1822 Raices Valores Negociables</t>
+          <t>Alpha Mega</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>27202.22</v>
+        <v>538018.11</v>
+      </c>
+      <c r="C4" t="n">
+        <v>534458.55</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Alpha Acciones</t>
+          <t>Alpha Recursos Naturales</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>370309.86</v>
+        <v>268255.2</v>
+      </c>
+      <c r="C5" t="n">
+        <v>269384.72</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Alpha Mega</t>
+          <t>Alpha renta balan global</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>538018.11</v>
+        <v>124900.04</v>
+      </c>
+      <c r="C6" t="n">
+        <v>118364.76</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Alpha Recursos Naturales</t>
+          <t>Fima Acciones</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>268255.2</v>
+        <v>256290.21</v>
+      </c>
+      <c r="C7" t="n">
+        <v>253729.65</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Alpha renta balan global</t>
+          <t>Fima PB Acciones</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>124900.04</v>
+        <v>301155.97</v>
+      </c>
+      <c r="C8" t="n">
+        <v>303089.32</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Fima Acciones</t>
+          <t>HF Acciones Argentinas</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>256290.21</v>
+        <v>9540.9</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Fima PB Acciones</t>
+          <t>HF Acciones Lideres</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>301155.97</v>
+        <v>138994.33</v>
+      </c>
+      <c r="C10" t="n">
+        <v>139293</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>HF Acciones Argentinas</t>
+          <t>avg</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>9540.9</v>
+        <v>226074.09</v>
+      </c>
+      <c r="C11" t="n">
+        <v>223679.56</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>HF Acciones Lideres</t>
+          <t>total</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>138994.33</v>
+        <v>2034666.84</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2013116.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>